<commit_message>
CIERRE 10 NOV 2023
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/REPORTE  NOTAS CENTRAL  OCT-23.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/REPORTE  NOTAS CENTRAL  OCT-23.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="23865" windowHeight="11130" firstSheet="2" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="23865" windowHeight="11130" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="NOTAS  CENTRAL 16  al  21 Oct  " sheetId="1" r:id="rId1"/>
@@ -1834,6 +1834,9 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="15" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1923,9 +1926,6 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="15" fontId="2" fillId="11" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1936,11 +1936,11 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FF33CCFF"/>
+      <color rgb="FFCC99FF"/>
       <color rgb="FF66FF99"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FFCCFFCC"/>
-      <color rgb="FF33CCFF"/>
-      <color rgb="FFCC99FF"/>
       <color rgb="FF0000FF"/>
     </mruColors>
   </colors>
@@ -2012,15 +2012,15 @@
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
       <xdr:col>8</xdr:col>
-      <xdr:colOff>66675</xdr:colOff>
+      <xdr:colOff>447675</xdr:colOff>
       <xdr:row>0</xdr:row>
-      <xdr:rowOff>38100</xdr:rowOff>
+      <xdr:rowOff>333375</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>16</xdr:col>
-      <xdr:colOff>360831</xdr:colOff>
+      <xdr:colOff>741831</xdr:colOff>
       <xdr:row>42</xdr:row>
-      <xdr:rowOff>55685</xdr:rowOff>
+      <xdr:rowOff>93785</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -2040,7 +2040,7 @@
       </xdr:blipFill>
       <xdr:spPr bwMode="auto">
         <a:xfrm>
-          <a:off x="5524500" y="38100"/>
+          <a:off x="5972175" y="333375"/>
           <a:ext cx="6171081" cy="9275885"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -2375,8 +2375,8 @@
   </sheetPr>
   <dimension ref="B1:M47"/>
   <sheetViews>
-    <sheetView topLeftCell="A26" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F35" sqref="F35"/>
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection sqref="A1:N48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -2395,20 +2395,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="158" t="s">
+      <c r="C1" s="159" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
       <c r="I1" s="68"/>
-      <c r="J1" s="159" t="s">
+      <c r="J1" s="160" t="s">
         <v>191</v>
       </c>
-      <c r="K1" s="159"/>
-      <c r="L1" s="159"/>
-      <c r="M1" s="159"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
     </row>
     <row r="2" spans="2:13" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="43" t="s">
@@ -3340,8 +3340,8 @@
       </c>
       <c r="G32" s="27"/>
       <c r="I32" s="68"/>
-      <c r="J32" s="160"/>
-      <c r="K32" s="160"/>
+      <c r="J32" s="161"/>
+      <c r="K32" s="161"/>
       <c r="L32" s="150"/>
       <c r="M32" s="151"/>
     </row>
@@ -3429,10 +3429,10 @@
       <c r="G36" s="25"/>
       <c r="I36" s="68"/>
       <c r="K36" s="99"/>
-      <c r="L36" s="163" t="s">
+      <c r="L36" s="164" t="s">
         <v>210</v>
       </c>
-      <c r="M36" s="161">
+      <c r="M36" s="162">
         <f>F47-M31</f>
         <v>1037858.16</v>
       </c>
@@ -3456,8 +3456,8 @@
       <c r="G37" s="45"/>
       <c r="I37" s="68"/>
       <c r="K37" s="99"/>
-      <c r="L37" s="164"/>
-      <c r="M37" s="162"/>
+      <c r="L37" s="165"/>
+      <c r="M37" s="163"/>
     </row>
     <row r="38" spans="2:13" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
@@ -3522,10 +3522,10 @@
       <c r="G40" s="25"/>
       <c r="I40" s="68"/>
       <c r="K40" s="86"/>
-      <c r="L40" s="154" t="s">
+      <c r="L40" s="155" t="s">
         <v>209</v>
       </c>
-      <c r="M40" s="155"/>
+      <c r="M40" s="156"/>
     </row>
     <row r="41" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="6">
@@ -3545,8 +3545,8 @@
       </c>
       <c r="G41" s="25"/>
       <c r="I41" s="68"/>
-      <c r="L41" s="156"/>
-      <c r="M41" s="157"/>
+      <c r="L41" s="157"/>
+      <c r="M41" s="158"/>
     </row>
     <row r="42" spans="2:13" ht="16.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B42" s="6">
@@ -3685,19 +3685,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="158" t="s">
+      <c r="C1" s="159" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-      <c r="J1" s="159" t="s">
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
+      <c r="J1" s="160" t="s">
         <v>202</v>
       </c>
-      <c r="K1" s="159"/>
-      <c r="L1" s="159"/>
-      <c r="M1" s="159"/>
+      <c r="K1" s="160"/>
+      <c r="L1" s="160"/>
+      <c r="M1" s="160"/>
     </row>
     <row r="2" spans="2:13" ht="41.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
@@ -4880,10 +4880,10 @@
       </c>
       <c r="J39" s="86"/>
       <c r="K39" s="95"/>
-      <c r="L39" s="165" t="s">
+      <c r="L39" s="166" t="s">
         <v>210</v>
       </c>
-      <c r="M39" s="167">
+      <c r="M39" s="168">
         <f>F43-M37</f>
         <v>225360.95000000007</v>
       </c>
@@ -4908,8 +4908,8 @@
         <v>190</v>
       </c>
       <c r="K40" s="94"/>
-      <c r="L40" s="166"/>
-      <c r="M40" s="168"/>
+      <c r="L40" s="167"/>
+      <c r="M40" s="169"/>
     </row>
     <row r="41" spans="2:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6">
@@ -4971,15 +4971,15 @@
   <sheetPr>
     <tabColor rgb="FFCCFFCC"/>
   </sheetPr>
-  <dimension ref="B1:N48"/>
+  <dimension ref="B1:O49"/>
   <sheetViews>
-    <sheetView topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="E44" sqref="E44"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="V18" sqref="V18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="3.85546875" customWidth="1"/>
+    <col min="1" max="1" width="12.42578125" customWidth="1"/>
     <col min="2" max="2" width="4.42578125" customWidth="1"/>
     <col min="3" max="3" width="13.42578125" customWidth="1"/>
     <col min="4" max="4" width="11.5703125" style="2" customWidth="1"/>
@@ -4991,385 +4991,367 @@
     <col min="13" max="13" width="11.42578125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="2:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="158" t="s">
+    <row r="1" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C2" s="159" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
-    </row>
-    <row r="2" spans="2:8" ht="57" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="43" t="s">
+      <c r="D2" s="159"/>
+      <c r="E2" s="159"/>
+      <c r="F2" s="159"/>
+      <c r="G2" s="159"/>
+    </row>
+    <row r="3" spans="2:8" ht="57" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C3" s="43" t="s">
         <v>0</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D3" s="21" t="s">
         <v>71</v>
       </c>
-      <c r="E2" s="23" t="s">
+      <c r="E3" s="23" t="s">
         <v>72</v>
       </c>
-      <c r="F2" s="19" t="s">
+      <c r="F3" s="19" t="s">
         <v>1</v>
       </c>
-      <c r="G2" s="129"/>
-      <c r="H2" s="68"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B3" s="6">
-        <v>1</v>
-      </c>
-      <c r="C3" s="102">
-        <v>45222</v>
-      </c>
-      <c r="D3" s="103" t="s">
-        <v>211</v>
-      </c>
-      <c r="E3" s="106" t="s">
-        <v>103</v>
-      </c>
-      <c r="F3" s="104">
-        <v>22751.1</v>
-      </c>
-      <c r="G3" s="130"/>
+      <c r="G3" s="129"/>
       <c r="H3" s="68"/>
     </row>
     <row r="4" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B4" s="6">
-        <v>2</v>
-      </c>
-      <c r="C4" s="32">
+        <v>1</v>
+      </c>
+      <c r="C4" s="102">
         <v>45222</v>
       </c>
-      <c r="D4" s="105" t="s">
-        <v>212</v>
-      </c>
-      <c r="E4" s="28" t="s">
-        <v>104</v>
-      </c>
-      <c r="F4" s="33">
-        <v>70164.84</v>
-      </c>
-      <c r="G4" s="131"/>
+      <c r="D4" s="103" t="s">
+        <v>211</v>
+      </c>
+      <c r="E4" s="106" t="s">
+        <v>103</v>
+      </c>
+      <c r="F4" s="104">
+        <v>22751.1</v>
+      </c>
+      <c r="G4" s="130"/>
       <c r="H4" s="68"/>
     </row>
     <row r="5" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B5" s="6">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="C5" s="32">
         <v>45222</v>
       </c>
       <c r="D5" s="105" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="E5" s="28" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="F5" s="33">
-        <v>20764.400000000001</v>
+        <v>70164.84</v>
       </c>
       <c r="G5" s="131"/>
       <c r="H5" s="68"/>
     </row>
-    <row r="6" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="6" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B6" s="6">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="C6" s="32">
         <v>45222</v>
       </c>
       <c r="D6" s="105" t="s">
-        <v>51</v>
+        <v>213</v>
       </c>
       <c r="E6" s="28" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="F6" s="33">
-        <v>18512.5</v>
-      </c>
-      <c r="G6" s="132"/>
+        <v>20764.400000000001</v>
+      </c>
+      <c r="G6" s="131"/>
       <c r="H6" s="68"/>
     </row>
-    <row r="7" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B7" s="6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="C7" s="32">
         <v>45222</v>
       </c>
       <c r="D7" s="105" t="s">
+        <v>51</v>
+      </c>
+      <c r="E7" s="28" t="s">
+        <v>106</v>
+      </c>
+      <c r="F7" s="33">
+        <v>18512.5</v>
+      </c>
+      <c r="G7" s="132"/>
+      <c r="H7" s="68"/>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.25">
+      <c r="B8" s="6">
+        <v>5</v>
+      </c>
+      <c r="C8" s="32">
+        <v>45222</v>
+      </c>
+      <c r="D8" s="105" t="s">
         <v>52</v>
       </c>
-      <c r="E7" s="28" t="s">
+      <c r="E8" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="F7" s="33">
+      <c r="F8" s="33">
         <v>5100.8</v>
-      </c>
-      <c r="G7" s="131"/>
-      <c r="H7" s="68"/>
-    </row>
-    <row r="8" spans="2:8" ht="21" x14ac:dyDescent="0.35">
-      <c r="B8" s="6">
-        <v>6</v>
-      </c>
-      <c r="C8" s="184">
-        <v>45220</v>
-      </c>
-      <c r="D8" s="105" t="s">
-        <v>53</v>
-      </c>
-      <c r="E8" s="107" t="s">
-        <v>115</v>
-      </c>
-      <c r="F8" s="33">
-        <v>6076.2</v>
       </c>
       <c r="G8" s="131"/>
       <c r="H8" s="68"/>
     </row>
-    <row r="9" spans="2:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:8" ht="21" x14ac:dyDescent="0.35">
       <c r="B9" s="6">
-        <v>7</v>
-      </c>
-      <c r="C9" s="32">
-        <v>45222</v>
+        <v>6</v>
+      </c>
+      <c r="C9" s="154">
+        <v>45220</v>
       </c>
       <c r="D9" s="105" t="s">
-        <v>54</v>
-      </c>
-      <c r="E9" s="30" t="s">
-        <v>120</v>
+        <v>53</v>
+      </c>
+      <c r="E9" s="107" t="s">
+        <v>115</v>
       </c>
       <c r="F9" s="33">
-        <v>2436</v>
+        <v>6076.2</v>
       </c>
       <c r="G9" s="131"/>
       <c r="H9" s="68"/>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B10" s="6">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="C10" s="32">
         <v>45222</v>
       </c>
       <c r="D10" s="105" t="s">
-        <v>60</v>
+        <v>54</v>
       </c>
       <c r="E10" s="30" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F10" s="33">
-        <v>9656</v>
+        <v>2436</v>
       </c>
       <c r="G10" s="131"/>
       <c r="H10" s="68"/>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B11" s="6">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="C11" s="32">
         <v>45222</v>
       </c>
       <c r="D11" s="105" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="E11" s="30" t="s">
-        <v>215</v>
+        <v>121</v>
       </c>
       <c r="F11" s="33">
-        <v>48937.4</v>
+        <v>9656</v>
       </c>
       <c r="G11" s="131"/>
       <c r="H11" s="68"/>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B12" s="6">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C12" s="32">
-        <v>45223</v>
+        <v>45222</v>
       </c>
       <c r="D12" s="105" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
       <c r="E12" s="30" t="s">
-        <v>122</v>
+        <v>215</v>
       </c>
       <c r="F12" s="33">
-        <v>67869.600000000006</v>
+        <v>48937.4</v>
       </c>
       <c r="G12" s="131"/>
       <c r="H12" s="68"/>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B13" s="6">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C13" s="32">
         <v>45223</v>
       </c>
       <c r="D13" s="105" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
       <c r="E13" s="30" t="s">
-        <v>110</v>
+        <v>122</v>
       </c>
       <c r="F13" s="33">
-        <v>15440</v>
-      </c>
-      <c r="G13" s="133"/>
+        <v>67869.600000000006</v>
+      </c>
+      <c r="G13" s="131"/>
       <c r="H13" s="68"/>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B14" s="6">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="C14" s="32">
         <v>45223</v>
       </c>
       <c r="D14" s="105" t="s">
-        <v>64</v>
-      </c>
-      <c r="E14" s="28" t="s">
-        <v>123</v>
+        <v>63</v>
+      </c>
+      <c r="E14" s="30" t="s">
+        <v>110</v>
       </c>
       <c r="F14" s="33">
-        <v>26845.200000000001</v>
-      </c>
-      <c r="G14" s="131"/>
+        <v>15440</v>
+      </c>
+      <c r="G14" s="133"/>
       <c r="H14" s="68"/>
     </row>
     <row r="15" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B15" s="6">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C15" s="32">
         <v>45223</v>
       </c>
       <c r="D15" s="105" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E15" s="28" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F15" s="33">
-        <v>606</v>
+        <v>26845.200000000001</v>
       </c>
       <c r="G15" s="131"/>
       <c r="H15" s="68"/>
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B16" s="6">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C16" s="32">
-        <v>45224</v>
+        <v>45223</v>
       </c>
       <c r="D16" s="105" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E16" s="28" t="s">
-        <v>153</v>
+        <v>124</v>
       </c>
       <c r="F16" s="33">
-        <v>55687.5</v>
+        <v>606</v>
       </c>
       <c r="G16" s="131"/>
       <c r="H16" s="68"/>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B17" s="6">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="C17" s="32">
         <v>45224</v>
       </c>
       <c r="D17" s="105" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E17" s="28" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="F17" s="33">
-        <v>10019.6</v>
+        <v>55687.5</v>
       </c>
       <c r="G17" s="131"/>
       <c r="H17" s="68"/>
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B18" s="6">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C18" s="32">
         <v>45224</v>
       </c>
       <c r="D18" s="105" t="s">
-        <v>130</v>
+        <v>67</v>
       </c>
       <c r="E18" s="28" t="s">
-        <v>158</v>
+        <v>155</v>
       </c>
       <c r="F18" s="33">
-        <v>134020.35999999999</v>
+        <v>10019.6</v>
       </c>
       <c r="G18" s="131"/>
       <c r="H18" s="68"/>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B19" s="6">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C19" s="32">
         <v>45224</v>
       </c>
       <c r="D19" s="105" t="s">
-        <v>131</v>
-      </c>
-      <c r="E19" s="30" t="s">
-        <v>159</v>
+        <v>130</v>
+      </c>
+      <c r="E19" s="28" t="s">
+        <v>158</v>
       </c>
       <c r="F19" s="33">
-        <v>6188</v>
+        <v>134020.35999999999</v>
       </c>
       <c r="G19" s="131"/>
       <c r="H19" s="68"/>
     </row>
     <row r="20" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B20" s="6">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C20" s="32">
-        <v>45223</v>
+        <v>45224</v>
       </c>
       <c r="D20" s="105" t="s">
-        <v>132</v>
+        <v>131</v>
       </c>
       <c r="E20" s="30" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="F20" s="33">
-        <v>0</v>
+        <v>6188</v>
       </c>
       <c r="G20" s="131"/>
       <c r="H20" s="68"/>
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B21" s="6">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="C21" s="32">
-        <v>45224</v>
+        <v>45223</v>
       </c>
       <c r="D21" s="105" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="E21" s="30" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="F21" s="33">
         <v>0</v>
@@ -5379,450 +5361,477 @@
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B22" s="6">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="C22" s="32">
-        <v>45225</v>
+        <v>45224</v>
       </c>
       <c r="D22" s="105" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E22" s="30" t="s">
-        <v>162</v>
+        <v>159</v>
       </c>
       <c r="F22" s="33">
-        <v>124407.5</v>
+        <v>0</v>
       </c>
       <c r="G22" s="131"/>
       <c r="H22" s="68"/>
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B23" s="6">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="C23" s="32">
         <v>45225</v>
       </c>
       <c r="D23" s="105" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E23" s="30" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="F23" s="33">
-        <v>10456.44</v>
+        <v>124407.5</v>
       </c>
       <c r="G23" s="131"/>
       <c r="H23" s="68"/>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B24" s="6">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C24" s="32">
         <v>45225</v>
       </c>
       <c r="D24" s="105" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="E24" s="30" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="F24" s="33">
-        <v>345</v>
-      </c>
-      <c r="G24" s="133"/>
+        <v>10456.44</v>
+      </c>
+      <c r="G24" s="131"/>
       <c r="H24" s="68"/>
     </row>
     <row r="25" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B25" s="6">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="C25" s="32">
         <v>45225</v>
       </c>
       <c r="D25" s="105" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="E25" s="30" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="F25" s="33">
-        <v>45834.7</v>
-      </c>
-      <c r="G25" s="131"/>
+        <v>345</v>
+      </c>
+      <c r="G25" s="133"/>
       <c r="H25" s="68"/>
     </row>
     <row r="26" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B26" s="6">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="C26" s="32">
         <v>45225</v>
       </c>
       <c r="D26" s="105" t="s">
-        <v>138</v>
-      </c>
-      <c r="E26" s="28" t="s">
-        <v>167</v>
+        <v>137</v>
+      </c>
+      <c r="E26" s="30" t="s">
+        <v>165</v>
       </c>
       <c r="F26" s="33">
-        <v>7125</v>
+        <v>45834.7</v>
       </c>
       <c r="G26" s="131"/>
       <c r="H26" s="68"/>
     </row>
     <row r="27" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B27" s="6">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C27" s="32">
         <v>45225</v>
       </c>
       <c r="D27" s="105" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E27" s="28" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="F27" s="33">
-        <v>55137.9</v>
+        <v>7125</v>
       </c>
       <c r="G27" s="131"/>
       <c r="H27" s="68"/>
     </row>
     <row r="28" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B28" s="6">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C28" s="32">
-        <v>45226</v>
+        <v>45225</v>
       </c>
       <c r="D28" s="105" t="s">
-        <v>140</v>
-      </c>
-      <c r="E28" s="30" t="s">
-        <v>168</v>
+        <v>139</v>
+      </c>
+      <c r="E28" s="28" t="s">
+        <v>166</v>
       </c>
       <c r="F28" s="33">
-        <v>37652.400000000001</v>
+        <v>55137.9</v>
       </c>
       <c r="G28" s="131"/>
       <c r="H28" s="68"/>
     </row>
     <row r="29" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B29" s="6">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C29" s="32">
         <v>45226</v>
       </c>
       <c r="D29" s="105" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="E29" s="30" t="s">
-        <v>171</v>
+        <v>168</v>
       </c>
       <c r="F29" s="33">
-        <v>48202.54</v>
+        <v>37652.400000000001</v>
       </c>
       <c r="G29" s="131"/>
       <c r="H29" s="68"/>
     </row>
     <row r="30" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B30" s="6">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C30" s="32">
         <v>45226</v>
       </c>
       <c r="D30" s="105" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="E30" s="30" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="F30" s="33">
-        <v>5609.2</v>
+        <v>48202.54</v>
       </c>
       <c r="G30" s="131"/>
       <c r="H30" s="68"/>
     </row>
-    <row r="31" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="31" spans="2:8" x14ac:dyDescent="0.25">
       <c r="B31" s="6">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C31" s="32">
         <v>45226</v>
       </c>
       <c r="D31" s="105" t="s">
+        <v>142</v>
+      </c>
+      <c r="E31" s="30" t="s">
+        <v>156</v>
+      </c>
+      <c r="F31" s="33">
+        <v>5609.2</v>
+      </c>
+      <c r="G31" s="131"/>
+      <c r="H31" s="68"/>
+    </row>
+    <row r="32" spans="2:8" ht="18.75" x14ac:dyDescent="0.3">
+      <c r="B32" s="6">
+        <v>29</v>
+      </c>
+      <c r="C32" s="32">
+        <v>45226</v>
+      </c>
+      <c r="D32" s="105" t="s">
         <v>143</v>
       </c>
-      <c r="E31" s="30" t="s">
+      <c r="E32" s="30" t="s">
         <v>180</v>
       </c>
-      <c r="F31" s="33">
+      <c r="F32" s="33">
         <v>43436.800000000003</v>
       </c>
-      <c r="G31" s="132"/>
-      <c r="H31" s="68"/>
-    </row>
-    <row r="32" spans="2:8" x14ac:dyDescent="0.25">
-      <c r="B32" s="6">
+      <c r="G32" s="132"/>
+      <c r="H32" s="68"/>
+    </row>
+    <row r="33" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B33" s="6">
         <v>30</v>
-      </c>
-      <c r="C32" s="32">
-        <v>45227</v>
-      </c>
-      <c r="D32" s="105" t="s">
-        <v>144</v>
-      </c>
-      <c r="E32" s="30" t="s">
-        <v>172</v>
-      </c>
-      <c r="F32" s="33">
-        <v>199527.8</v>
-      </c>
-      <c r="G32" s="134"/>
-      <c r="H32" s="68"/>
-    </row>
-    <row r="33" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B33" s="6">
-        <v>31</v>
       </c>
       <c r="C33" s="32">
         <v>45227</v>
       </c>
       <c r="D33" s="105" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="E33" s="30" t="s">
-        <v>173</v>
+        <v>172</v>
       </c>
       <c r="F33" s="33">
-        <v>29534.1</v>
-      </c>
-      <c r="G33" s="135"/>
+        <v>199527.8</v>
+      </c>
+      <c r="G33" s="134"/>
       <c r="H33" s="68"/>
     </row>
-    <row r="34" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B34" s="6">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C34" s="32">
         <v>45227</v>
       </c>
       <c r="D34" s="105" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="E34" s="30" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="F34" s="33">
-        <v>1734.4</v>
-      </c>
-      <c r="G34" s="131"/>
+        <v>29534.1</v>
+      </c>
+      <c r="G34" s="135"/>
       <c r="H34" s="68"/>
     </row>
-    <row r="35" spans="2:14" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="6">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C35" s="32">
         <v>45227</v>
       </c>
       <c r="D35" s="105" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="E35" s="30" t="s">
-        <v>181</v>
+        <v>174</v>
       </c>
       <c r="F35" s="33">
-        <v>17967.2</v>
-      </c>
-      <c r="G35" s="132"/>
+        <v>1734.4</v>
+      </c>
+      <c r="G35" s="131"/>
       <c r="H35" s="68"/>
     </row>
-    <row r="36" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:15" ht="18.75" x14ac:dyDescent="0.3">
       <c r="B36" s="6">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C36" s="32">
         <v>45227</v>
       </c>
       <c r="D36" s="105" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="E36" s="30" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="F36" s="33">
-        <v>640</v>
-      </c>
-      <c r="G36" s="133"/>
+        <v>17967.2</v>
+      </c>
+      <c r="G36" s="132"/>
       <c r="H36" s="68"/>
     </row>
-    <row r="37" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B37" s="6">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C37" s="32">
         <v>45227</v>
       </c>
       <c r="D37" s="105" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="E37" s="30" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="F37" s="33">
-        <v>7296</v>
-      </c>
-      <c r="G37" s="136"/>
+        <v>640</v>
+      </c>
+      <c r="G37" s="133"/>
       <c r="H37" s="68"/>
     </row>
-    <row r="38" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C38" s="32">
         <v>45227</v>
       </c>
       <c r="D38" s="105" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="E38" s="30" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="F38" s="33">
-        <v>17830.3</v>
-      </c>
-      <c r="G38" s="133"/>
+        <v>7296</v>
+      </c>
+      <c r="G38" s="136"/>
       <c r="H38" s="68"/>
     </row>
-    <row r="39" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B39" s="6">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C39" s="32">
         <v>45227</v>
       </c>
       <c r="D39" s="105" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="E39" s="30" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="F39" s="33">
-        <v>1211.4000000000001</v>
+        <v>17830.3</v>
       </c>
       <c r="G39" s="133"/>
       <c r="H39" s="68"/>
     </row>
-    <row r="40" spans="2:14" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B40" s="6">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C40" s="32">
         <v>45227</v>
       </c>
       <c r="D40" s="105" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="E40" s="30" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="F40" s="33">
-        <v>20743.599999999999</v>
+        <v>1211.4000000000001</v>
       </c>
       <c r="G40" s="133"/>
       <c r="H40" s="68"/>
     </row>
-    <row r="41" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="B41" s="12"/>
-      <c r="C41" s="111"/>
-      <c r="D41" s="40"/>
-      <c r="E41" s="41"/>
-      <c r="F41" s="42"/>
-      <c r="G41" s="138"/>
+    <row r="41" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B41" s="6">
+        <v>38</v>
+      </c>
+      <c r="C41" s="32">
+        <v>45227</v>
+      </c>
+      <c r="D41" s="105" t="s">
+        <v>152</v>
+      </c>
+      <c r="E41" s="30" t="s">
+        <v>186</v>
+      </c>
+      <c r="F41" s="33">
+        <v>20743.599999999999</v>
+      </c>
+      <c r="G41" s="133"/>
       <c r="H41" s="68"/>
     </row>
-    <row r="42" spans="2:14" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="B42" s="114"/>
-      <c r="C42" s="113"/>
-      <c r="D42" s="124" t="s">
-        <v>69</v>
-      </c>
-      <c r="E42" s="125"/>
-      <c r="F42" s="126">
-        <f>SUM(F3:F41)</f>
-        <v>1195767.78</v>
-      </c>
-      <c r="H42" s="137"/>
-    </row>
-    <row r="43" spans="2:14" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="42" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="B42" s="12"/>
+      <c r="C42" s="111"/>
+      <c r="D42" s="40"/>
+      <c r="E42" s="41"/>
+      <c r="F42" s="42"/>
+      <c r="G42" s="138"/>
+      <c r="H42" s="68"/>
+    </row>
+    <row r="43" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B43" s="114"/>
       <c r="C43" s="113"/>
-      <c r="D43" s="114"/>
-      <c r="E43" s="115"/>
-      <c r="F43" s="116"/>
-      <c r="G43" s="121"/>
-      <c r="H43" s="110"/>
-      <c r="J43" s="99"/>
-      <c r="K43" s="100"/>
-      <c r="L43" s="100"/>
-      <c r="M43" s="100"/>
-      <c r="N43" s="100"/>
-    </row>
-    <row r="44" spans="2:14" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="B44" s="2"/>
-      <c r="F44" s="171" t="s">
+      <c r="D43" s="124" t="s">
+        <v>69</v>
+      </c>
+      <c r="E43" s="125"/>
+      <c r="F43" s="126">
+        <f>SUM(F4:F42)</f>
+        <v>1195767.78</v>
+      </c>
+      <c r="H43" s="137"/>
+    </row>
+    <row r="44" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="B44" s="114"/>
+      <c r="C44" s="113"/>
+      <c r="D44" s="114"/>
+      <c r="E44" s="115"/>
+      <c r="F44" s="116"/>
+      <c r="G44" s="121"/>
+      <c r="H44" s="110"/>
+      <c r="I44" s="100"/>
+      <c r="J44" s="99"/>
+      <c r="K44" s="100"/>
+      <c r="L44" s="100"/>
+      <c r="M44" s="100"/>
+      <c r="N44" s="100"/>
+      <c r="O44" s="100"/>
+    </row>
+    <row r="45" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="B45" s="2"/>
+      <c r="F45" s="172" t="s">
         <v>221</v>
       </c>
-      <c r="G44" s="172"/>
-      <c r="H44" s="173"/>
-      <c r="J44" s="169" t="s">
+      <c r="G45" s="173"/>
+      <c r="H45" s="174"/>
+      <c r="I45" s="100"/>
+      <c r="J45" s="170" t="s">
         <v>210</v>
       </c>
-      <c r="K44" s="170"/>
-      <c r="L44" s="177">
-        <f>F42-982143.23</f>
+      <c r="K45" s="171"/>
+      <c r="L45" s="178">
+        <f>F43-982143.23</f>
         <v>213624.55000000005</v>
       </c>
-      <c r="M44" s="178"/>
-      <c r="N44" s="178"/>
-    </row>
-    <row r="45" spans="2:14" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F45" s="174"/>
-      <c r="G45" s="175"/>
-      <c r="H45" s="176"/>
-      <c r="J45" s="169"/>
-      <c r="K45" s="170"/>
-      <c r="L45" s="177"/>
-      <c r="M45" s="178"/>
-      <c r="N45" s="178"/>
-    </row>
-    <row r="46" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J46" s="99"/>
-      <c r="K46" s="101"/>
-      <c r="L46" s="101"/>
-      <c r="M46" s="100"/>
-      <c r="N46" s="100"/>
-    </row>
-    <row r="47" spans="2:14" x14ac:dyDescent="0.25">
-      <c r="J47" s="86"/>
-      <c r="K47" s="87"/>
-      <c r="L47" s="87"/>
-    </row>
-    <row r="48" spans="2:14" x14ac:dyDescent="0.25">
+      <c r="M45" s="179"/>
+      <c r="N45" s="179"/>
+      <c r="O45" s="100"/>
+    </row>
+    <row r="46" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="F46" s="175"/>
+      <c r="G46" s="176"/>
+      <c r="H46" s="177"/>
+      <c r="I46" s="100"/>
+      <c r="J46" s="170"/>
+      <c r="K46" s="171"/>
+      <c r="L46" s="178"/>
+      <c r="M46" s="179"/>
+      <c r="N46" s="179"/>
+      <c r="O46" s="100"/>
+    </row>
+    <row r="47" spans="2:15" x14ac:dyDescent="0.25">
+      <c r="I47" s="100"/>
+      <c r="J47" s="99"/>
+      <c r="K47" s="101"/>
+      <c r="L47" s="101"/>
+      <c r="M47" s="100"/>
+      <c r="N47" s="100"/>
+      <c r="O47" s="100"/>
+    </row>
+    <row r="48" spans="2:15" x14ac:dyDescent="0.25">
       <c r="J48" s="86"/>
+      <c r="K48" s="87"/>
+      <c r="L48" s="87"/>
+    </row>
+    <row r="49" spans="10:10" x14ac:dyDescent="0.25">
+      <c r="J49" s="86"/>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="C1:G1"/>
-    <mergeCell ref="J44:K45"/>
-    <mergeCell ref="F44:H45"/>
-    <mergeCell ref="L44:N45"/>
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="J45:K46"/>
+    <mergeCell ref="F45:H46"/>
+    <mergeCell ref="L45:N46"/>
   </mergeCells>
   <pageMargins left="0.19685039370078741" right="0.11811023622047245" top="0.27559055118110237" bottom="0.27559055118110237" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="73" orientation="landscape" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -5837,7 +5846,7 @@
   </sheetPr>
   <dimension ref="B1:G47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A13" zoomScaleNormal="100" workbookViewId="0">
+    <sheetView topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
       <selection activeCell="H38" sqref="H38"/>
     </sheetView>
   </sheetViews>
@@ -5855,13 +5864,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="158" t="s">
+      <c r="C1" s="159" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="158"/>
-      <c r="E1" s="158"/>
-      <c r="F1" s="158"/>
-      <c r="G1" s="158"/>
+      <c r="D1" s="159"/>
+      <c r="E1" s="159"/>
+      <c r="F1" s="159"/>
+      <c r="G1" s="159"/>
     </row>
     <row r="2" spans="2:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="43" t="s">
@@ -6404,23 +6413,23 @@
     </row>
     <row r="34" spans="2:7" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="112"/>
-      <c r="C34" s="183" t="s">
+      <c r="C34" s="184" t="s">
         <v>210</v>
       </c>
-      <c r="D34" s="183"/>
-      <c r="E34" s="179">
+      <c r="D34" s="184"/>
+      <c r="E34" s="180">
         <f>F31-782498.42</f>
         <v>718019.03999999992</v>
       </c>
-      <c r="F34" s="180"/>
+      <c r="F34" s="181"/>
       <c r="G34" s="117"/>
     </row>
     <row r="35" spans="2:7" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="112"/>
-      <c r="C35" s="183"/>
-      <c r="D35" s="183"/>
-      <c r="E35" s="181"/>
-      <c r="F35" s="182"/>
+      <c r="C35" s="184"/>
+      <c r="D35" s="184"/>
+      <c r="E35" s="182"/>
+      <c r="F35" s="183"/>
       <c r="G35" s="118"/>
     </row>
     <row r="36" spans="2:7" ht="18.75" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
CIERRE 28 NOV 23
</commit_message>
<xml_diff>
--- a/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/REPORTE  NOTAS CENTRAL  OCT-23.xlsx
+++ b/01 DOCUEMENTOS/CENTRAL   ARCHIVO   2 0 2 3/REPORTE  NOTAS CENTRAL  OCT-23.xlsx
@@ -18,7 +18,7 @@
     <sheet name="OBRADOR &amp; CENTRAL 30-04-Nov" sheetId="4" r:id="rId4"/>
     <sheet name="OBRADOR &amp; CENTRAL 6-11 Nov-23" sheetId="5" r:id="rId5"/>
     <sheet name="OBRADOR &amp; CENTRAL  13-18-Noviem" sheetId="6" r:id="rId6"/>
-    <sheet name="Hoja3" sheetId="7" r:id="rId7"/>
+    <sheet name="OBRADOR  &amp; CENTRAL 18-25 Nov-23" sheetId="7" r:id="rId7"/>
     <sheet name="Hoja1" sheetId="8" r:id="rId8"/>
     <sheet name="Hoja2" sheetId="9" r:id="rId9"/>
   </sheets>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="791" uniqueCount="520">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="799" uniqueCount="530">
   <si>
     <t>FECHA</t>
   </si>
@@ -1592,6 +1592,36 @@
   </si>
   <si>
     <t>FALTA ORIGINAL OSIRIS</t>
+  </si>
+  <si>
+    <t>M-400</t>
+  </si>
+  <si>
+    <t>408 M</t>
+  </si>
+  <si>
+    <t>M-408</t>
+  </si>
+  <si>
+    <t>409 M</t>
+  </si>
+  <si>
+    <t>M-409</t>
+  </si>
+  <si>
+    <t>410 M</t>
+  </si>
+  <si>
+    <t>M-410</t>
+  </si>
+  <si>
+    <t xml:space="preserve">  </t>
+  </si>
+  <si>
+    <t>SEMANA DEL  18--25--Nov-23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SALIDAS  OBRADOR     A   CENTRAL  </t>
   </si>
 </sst>
 </file>
@@ -1601,7 +1631,7 @@
   <numFmts count="1">
     <numFmt numFmtId="44" formatCode="_-&quot;$&quot;* #,##0.00_-;\-&quot;$&quot;* #,##0.00_-;_-&quot;$&quot;* &quot;-&quot;??_-;_-@_-"/>
   </numFmts>
-  <fonts count="17" x14ac:knownFonts="1">
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1734,6 +1764,21 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="16">
     <fill>
@@ -2717,7 +2762,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="337">
+  <cellXfs count="338">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -3250,6 +3295,10 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="44" fontId="2" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="2" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" textRotation="34"/>
     </xf>
@@ -3349,60 +3398,60 @@
     <xf numFmtId="0" fontId="2" fillId="9" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="13" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="20" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="57" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="2" borderId="58" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="13" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="36" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="49" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="50" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="21" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="15" borderId="22" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="44" fontId="4" fillId="14" borderId="67" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3418,11 +3467,8 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="11" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="18" fillId="0" borderId="38" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Moneda" xfId="1" builtinId="4"/>
@@ -3432,6 +3478,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFF00FF"/>
       <color rgb="FFCC99FF"/>
       <color rgb="FFFFCCFF"/>
       <color rgb="FF33CCFF"/>
@@ -3439,7 +3486,6 @@
       <color rgb="FF66FF99"/>
       <color rgb="FF0000FF"/>
       <color rgb="FF99FF66"/>
-      <color rgb="FFFF00FF"/>
       <color rgb="FF99CCFF"/>
       <color rgb="FFCCFFCC"/>
     </mruColors>
@@ -3961,6 +4007,108 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing7.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>11</xdr:col>
+      <xdr:colOff>752475</xdr:colOff>
+      <xdr:row>0</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>20</xdr:col>
+      <xdr:colOff>657225</xdr:colOff>
+      <xdr:row>44</xdr:row>
+      <xdr:rowOff>171449</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="3" name="Imagen 2" descr="C:\Users\ROUSS\Pictures\2023-11-28 ESCANEO\CENTRAL &amp; OBRADOR  20-25 NOV-2023.jpg"/>
+        <xdr:cNvPicPr/>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId1" cstate="print">
+          <a:extLst>
+            <a:ext uri="{28A0092B-C50C-407E-A947-70E740481C1C}">
+              <a14:useLocalDpi xmlns:a14="http://schemas.microsoft.com/office/drawing/2010/main" val="0"/>
+            </a:ext>
+          </a:extLst>
+        </a:blip>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="8791575" y="76199"/>
+          <a:ext cx="6762750" cy="9572625"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>19052</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>152404</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>19</xdr:col>
+      <xdr:colOff>342900</xdr:colOff>
+      <xdr:row>40</xdr:row>
+      <xdr:rowOff>190500</xdr:rowOff>
+    </xdr:to>
+    <xdr:cxnSp macro="">
+      <xdr:nvCxnSpPr>
+        <xdr:cNvPr id="7" name="Conector angular 6"/>
+        <xdr:cNvCxnSpPr/>
+      </xdr:nvCxnSpPr>
+      <xdr:spPr>
+        <a:xfrm rot="10800000">
+          <a:off x="5657852" y="7639054"/>
+          <a:ext cx="8820148" cy="1142996"/>
+        </a:xfrm>
+        <a:prstGeom prst="bentConnector3">
+          <a:avLst>
+            <a:gd name="adj1" fmla="val 50000"/>
+          </a:avLst>
+        </a:prstGeom>
+        <a:ln>
+          <a:headEnd type="triangle"/>
+          <a:tailEnd type="triangle"/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="3">
+          <a:schemeClr val="accent2"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="2">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="tx1"/>
+        </a:fontRef>
+      </xdr:style>
+    </xdr:cxnSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
@@ -4249,20 +4397,20 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="285" t="s">
+      <c r="C1" s="287" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
       <c r="I1" s="68"/>
-      <c r="J1" s="286" t="s">
+      <c r="J1" s="288" t="s">
         <v>191</v>
       </c>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
+      <c r="K1" s="288"/>
+      <c r="L1" s="288"/>
+      <c r="M1" s="288"/>
     </row>
     <row r="2" spans="2:13" ht="33.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="43" t="s">
@@ -5194,8 +5342,8 @@
       </c>
       <c r="G32" s="27"/>
       <c r="I32" s="68"/>
-      <c r="J32" s="287"/>
-      <c r="K32" s="287"/>
+      <c r="J32" s="289"/>
+      <c r="K32" s="289"/>
       <c r="L32" s="147"/>
       <c r="M32" s="148"/>
     </row>
@@ -5253,7 +5401,7 @@
       <c r="D35" s="6" t="s">
         <v>37</v>
       </c>
-      <c r="E35" s="334" t="s">
+      <c r="E35" s="278" t="s">
         <v>467</v>
       </c>
       <c r="F35" s="8">
@@ -5285,10 +5433,10 @@
       <c r="G36" s="25"/>
       <c r="I36" s="68"/>
       <c r="K36" s="99"/>
-      <c r="L36" s="290" t="s">
+      <c r="L36" s="292" t="s">
         <v>210</v>
       </c>
-      <c r="M36" s="288">
+      <c r="M36" s="290">
         <f>F47-M31</f>
         <v>1037858.16</v>
       </c>
@@ -5312,8 +5460,8 @@
       <c r="G37" s="45"/>
       <c r="I37" s="68"/>
       <c r="K37" s="99"/>
-      <c r="L37" s="291"/>
-      <c r="M37" s="289"/>
+      <c r="L37" s="293"/>
+      <c r="M37" s="291"/>
     </row>
     <row r="38" spans="2:13" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B38" s="6">
@@ -5385,10 +5533,10 @@
       <c r="K40" s="157">
         <v>220000</v>
       </c>
-      <c r="L40" s="281" t="s">
+      <c r="L40" s="283" t="s">
         <v>209</v>
       </c>
-      <c r="M40" s="282"/>
+      <c r="M40" s="284"/>
     </row>
     <row r="41" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B41" s="6">
@@ -5416,8 +5564,8 @@
       <c r="K41" s="159">
         <v>25000</v>
       </c>
-      <c r="L41" s="283"/>
-      <c r="M41" s="284"/>
+      <c r="L41" s="285"/>
+      <c r="M41" s="286"/>
     </row>
     <row r="42" spans="2:13" ht="16.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B42" s="6">
@@ -5472,7 +5620,7 @@
       <c r="K43" s="159">
         <v>170000</v>
       </c>
-      <c r="L43" s="278" t="s">
+      <c r="L43" s="280" t="s">
         <v>280</v>
       </c>
       <c r="M43" s="166"/>
@@ -5503,7 +5651,7 @@
       <c r="K44" s="159">
         <v>180000</v>
       </c>
-      <c r="L44" s="279"/>
+      <c r="L44" s="281"/>
       <c r="M44" s="167"/>
     </row>
     <row r="45" spans="2:13" ht="13.5" customHeight="1" x14ac:dyDescent="0.25">
@@ -5532,7 +5680,7 @@
       <c r="K45" s="159">
         <v>60000</v>
       </c>
-      <c r="L45" s="279"/>
+      <c r="L45" s="281"/>
       <c r="M45" s="167"/>
     </row>
     <row r="46" spans="2:13" ht="21" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5551,7 +5699,7 @@
       <c r="K46" s="159">
         <v>98858</v>
       </c>
-      <c r="L46" s="279"/>
+      <c r="L46" s="281"/>
       <c r="M46" s="167"/>
     </row>
     <row r="47" spans="2:13" ht="24.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
@@ -5573,7 +5721,7 @@
       <c r="K47" s="163">
         <v>190000</v>
       </c>
-      <c r="L47" s="280"/>
+      <c r="L47" s="282"/>
       <c r="M47" s="168"/>
     </row>
     <row r="48" spans="2:13" x14ac:dyDescent="0.25">
@@ -5637,19 +5785,19 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:13" ht="40.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.5">
-      <c r="C1" s="285" t="s">
+      <c r="C1" s="287" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
-      <c r="J1" s="286" t="s">
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
+      <c r="J1" s="288" t="s">
         <v>202</v>
       </c>
-      <c r="K1" s="286"/>
-      <c r="L1" s="286"/>
-      <c r="M1" s="286"/>
+      <c r="K1" s="288"/>
+      <c r="L1" s="288"/>
+      <c r="M1" s="288"/>
     </row>
     <row r="2" spans="2:13" ht="41.25" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="1" t="s">
@@ -6832,10 +6980,10 @@
       </c>
       <c r="J39" s="86"/>
       <c r="K39" s="95"/>
-      <c r="L39" s="292" t="s">
+      <c r="L39" s="294" t="s">
         <v>210</v>
       </c>
-      <c r="M39" s="294">
+      <c r="M39" s="296">
         <f>F43-M37</f>
         <v>225360.95000000007</v>
       </c>
@@ -6860,8 +7008,8 @@
         <v>190</v>
       </c>
       <c r="K40" s="94"/>
-      <c r="L40" s="293"/>
-      <c r="M40" s="295"/>
+      <c r="L40" s="295"/>
+      <c r="M40" s="297"/>
     </row>
     <row r="41" spans="2:13" ht="19.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B41" s="6">
@@ -6945,13 +7093,13 @@
   <sheetData>
     <row r="1" spans="2:8" ht="39.75" customHeight="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:8" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="285" t="s">
+      <c r="C2" s="287" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="285"/>
-      <c r="E2" s="285"/>
-      <c r="F2" s="285"/>
-      <c r="G2" s="285"/>
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287"/>
     </row>
     <row r="3" spans="2:8" ht="57" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="43" t="s">
@@ -7731,34 +7879,34 @@
     </row>
     <row r="45" spans="2:15" ht="19.5" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B45" s="2"/>
-      <c r="F45" s="298" t="s">
+      <c r="F45" s="300" t="s">
         <v>221</v>
       </c>
-      <c r="G45" s="299"/>
-      <c r="H45" s="300"/>
+      <c r="G45" s="301"/>
+      <c r="H45" s="302"/>
       <c r="I45" s="100"/>
-      <c r="J45" s="296" t="s">
+      <c r="J45" s="298" t="s">
         <v>210</v>
       </c>
-      <c r="K45" s="297"/>
-      <c r="L45" s="304">
+      <c r="K45" s="299"/>
+      <c r="L45" s="306">
         <f>F43-982143.23</f>
         <v>213624.55000000005</v>
       </c>
-      <c r="M45" s="305"/>
-      <c r="N45" s="305"/>
+      <c r="M45" s="307"/>
+      <c r="N45" s="307"/>
       <c r="O45" s="100"/>
     </row>
     <row r="46" spans="2:15" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="F46" s="301"/>
-      <c r="G46" s="302"/>
-      <c r="H46" s="303"/>
+      <c r="F46" s="303"/>
+      <c r="G46" s="304"/>
+      <c r="H46" s="305"/>
       <c r="I46" s="100"/>
-      <c r="J46" s="296"/>
-      <c r="K46" s="297"/>
-      <c r="L46" s="304"/>
-      <c r="M46" s="305"/>
-      <c r="N46" s="305"/>
+      <c r="J46" s="298"/>
+      <c r="K46" s="299"/>
+      <c r="L46" s="306"/>
+      <c r="M46" s="307"/>
+      <c r="N46" s="307"/>
       <c r="O46" s="100"/>
     </row>
     <row r="47" spans="2:15" x14ac:dyDescent="0.25">
@@ -7818,13 +7966,13 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:7" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C1" s="285" t="s">
+      <c r="C1" s="287" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="285"/>
-      <c r="E1" s="285"/>
-      <c r="F1" s="285"/>
-      <c r="G1" s="285"/>
+      <c r="D1" s="287"/>
+      <c r="E1" s="287"/>
+      <c r="F1" s="287"/>
+      <c r="G1" s="287"/>
     </row>
     <row r="2" spans="2:7" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C2" s="43" t="s">
@@ -8368,23 +8516,23 @@
     </row>
     <row r="34" spans="2:13" ht="21.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B34" s="112"/>
-      <c r="C34" s="310" t="s">
+      <c r="C34" s="312" t="s">
         <v>210</v>
       </c>
-      <c r="D34" s="310"/>
-      <c r="E34" s="306">
+      <c r="D34" s="312"/>
+      <c r="E34" s="308">
         <f>F31-782498.42</f>
         <v>718019.03999999992</v>
       </c>
-      <c r="F34" s="307"/>
+      <c r="F34" s="309"/>
       <c r="G34" s="170"/>
     </row>
     <row r="35" spans="2:13" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="112"/>
-      <c r="C35" s="310"/>
-      <c r="D35" s="310"/>
-      <c r="E35" s="308"/>
-      <c r="F35" s="309"/>
+      <c r="C35" s="312"/>
+      <c r="D35" s="312"/>
+      <c r="E35" s="310"/>
+      <c r="F35" s="311"/>
       <c r="G35" s="171"/>
     </row>
     <row r="36" spans="2:13" ht="18.75" x14ac:dyDescent="0.25">
@@ -8584,27 +8732,27 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:22" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="285" t="s">
+      <c r="C2" s="287" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="285"/>
-      <c r="E2" s="285"/>
-      <c r="F2" s="285"/>
-      <c r="G2" s="285"/>
-      <c r="K2" s="311" t="s">
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287"/>
+      <c r="K2" s="330" t="s">
         <v>330</v>
       </c>
-      <c r="L2" s="311"/>
-      <c r="M2" s="311"/>
-      <c r="N2" s="311"/>
-      <c r="O2" s="311"/>
-      <c r="R2" s="311" t="s">
+      <c r="L2" s="330"/>
+      <c r="M2" s="330"/>
+      <c r="N2" s="330"/>
+      <c r="O2" s="330"/>
+      <c r="R2" s="330" t="s">
         <v>330</v>
       </c>
-      <c r="S2" s="311"/>
-      <c r="T2" s="311"/>
-      <c r="U2" s="311"/>
-      <c r="V2" s="311"/>
+      <c r="S2" s="330"/>
+      <c r="T2" s="330"/>
+      <c r="U2" s="330"/>
+      <c r="V2" s="330"/>
     </row>
     <row r="3" spans="2:22" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="43" t="s">
@@ -10158,15 +10306,15 @@
     </row>
     <row r="35" spans="2:22" x14ac:dyDescent="0.25">
       <c r="B35" s="112"/>
-      <c r="C35" s="310" t="s">
+      <c r="C35" s="312" t="s">
         <v>210</v>
       </c>
-      <c r="D35" s="310"/>
-      <c r="E35" s="306">
+      <c r="D35" s="312"/>
+      <c r="E35" s="308">
         <f>F32-U52</f>
         <v>-681081.05999999982</v>
       </c>
-      <c r="F35" s="307"/>
+      <c r="F35" s="309"/>
       <c r="G35" s="170"/>
       <c r="J35" s="6">
         <v>32</v>
@@ -10203,10 +10351,10 @@
     </row>
     <row r="36" spans="2:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="112"/>
-      <c r="C36" s="310"/>
-      <c r="D36" s="310"/>
-      <c r="E36" s="308"/>
-      <c r="F36" s="309"/>
+      <c r="C36" s="312"/>
+      <c r="D36" s="312"/>
+      <c r="E36" s="310"/>
+      <c r="F36" s="311"/>
       <c r="G36" s="171"/>
       <c r="J36" s="6">
         <v>33</v>
@@ -10399,10 +10547,10 @@
       <c r="G41" s="230"/>
       <c r="J41" s="188"/>
       <c r="K41" s="189"/>
-      <c r="L41" s="312" t="s">
+      <c r="L41" s="313" t="s">
         <v>412</v>
       </c>
-      <c r="M41" s="313"/>
+      <c r="M41" s="314"/>
       <c r="N41" s="185">
         <f>SUM(N4:N40)</f>
         <v>1545672.14</v>
@@ -10497,13 +10645,13 @@
       </c>
       <c r="G44" s="230"/>
       <c r="K44" s="222"/>
-      <c r="L44" s="320" t="s">
+      <c r="L44" s="321" t="s">
         <v>466</v>
       </c>
-      <c r="M44" s="321"/>
-      <c r="N44" s="321"/>
-      <c r="O44" s="321"/>
-      <c r="P44" s="322"/>
+      <c r="M44" s="322"/>
+      <c r="N44" s="322"/>
+      <c r="O44" s="322"/>
+      <c r="P44" s="323"/>
       <c r="Q44" s="265">
         <v>41</v>
       </c>
@@ -10528,11 +10676,11 @@
         <v>0</v>
       </c>
       <c r="G45" s="230"/>
-      <c r="L45" s="323"/>
-      <c r="M45" s="324"/>
-      <c r="N45" s="324"/>
-      <c r="O45" s="324"/>
-      <c r="P45" s="325"/>
+      <c r="L45" s="324"/>
+      <c r="M45" s="325"/>
+      <c r="N45" s="325"/>
+      <c r="O45" s="325"/>
+      <c r="P45" s="326"/>
       <c r="Q45" s="266">
         <v>42</v>
       </c>
@@ -10558,11 +10706,11 @@
         <v>681080</v>
       </c>
       <c r="G46" s="230"/>
-      <c r="L46" s="323"/>
-      <c r="M46" s="324"/>
-      <c r="N46" s="324"/>
-      <c r="O46" s="324"/>
-      <c r="P46" s="325"/>
+      <c r="L46" s="324"/>
+      <c r="M46" s="325"/>
+      <c r="N46" s="325"/>
+      <c r="O46" s="325"/>
+      <c r="P46" s="326"/>
       <c r="Q46" s="265">
         <v>43</v>
       </c>
@@ -10587,11 +10735,11 @@
       <c r="E47" s="233"/>
       <c r="F47" s="234"/>
       <c r="G47" s="235"/>
-      <c r="L47" s="326"/>
-      <c r="M47" s="327"/>
-      <c r="N47" s="327"/>
-      <c r="O47" s="327"/>
-      <c r="P47" s="328"/>
+      <c r="L47" s="327"/>
+      <c r="M47" s="328"/>
+      <c r="N47" s="328"/>
+      <c r="O47" s="328"/>
+      <c r="P47" s="329"/>
       <c r="Q47" s="266">
         <v>44</v>
       </c>
@@ -10648,10 +10796,10 @@
     <row r="50" spans="17:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="Q50" s="186"/>
       <c r="R50" s="217"/>
-      <c r="S50" s="316" t="s">
+      <c r="S50" s="317" t="s">
         <v>414</v>
       </c>
-      <c r="T50" s="317"/>
+      <c r="T50" s="318"/>
       <c r="U50" s="218">
         <f>SUM(U4:U49)</f>
         <v>661176.16</v>
@@ -10659,10 +10807,10 @@
       <c r="V50" s="187"/>
     </row>
     <row r="51" spans="17:22" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="S51" s="314" t="s">
+      <c r="S51" s="315" t="s">
         <v>413</v>
       </c>
-      <c r="T51" s="315"/>
+      <c r="T51" s="316"/>
       <c r="U51" s="216">
         <f>N41</f>
         <v>1545672.14</v>
@@ -10670,10 +10818,10 @@
       <c r="V51" s="187"/>
     </row>
     <row r="52" spans="17:22" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="S52" s="318" t="s">
+      <c r="S52" s="319" t="s">
         <v>415</v>
       </c>
-      <c r="T52" s="319"/>
+      <c r="T52" s="320"/>
       <c r="U52" s="221">
         <f>U50+U51</f>
         <v>2206848.2999999998</v>
@@ -10689,16 +10837,16 @@
     <sortCondition ref="S46:S48"/>
   </sortState>
   <mergeCells count="10">
+    <mergeCell ref="C2:G2"/>
+    <mergeCell ref="C35:D36"/>
+    <mergeCell ref="E35:F36"/>
+    <mergeCell ref="K2:O2"/>
+    <mergeCell ref="R2:V2"/>
     <mergeCell ref="L41:M41"/>
     <mergeCell ref="S51:T51"/>
     <mergeCell ref="S50:T50"/>
     <mergeCell ref="S52:T52"/>
     <mergeCell ref="L44:P47"/>
-    <mergeCell ref="C2:G2"/>
-    <mergeCell ref="C35:D36"/>
-    <mergeCell ref="E35:F36"/>
-    <mergeCell ref="K2:O2"/>
-    <mergeCell ref="R2:V2"/>
   </mergeCells>
   <pageMargins left="0.59055118110236227" right="0.23622047244094491" top="0.35433070866141736" bottom="0.31496062992125984" header="0.31496062992125984" footer="0.31496062992125984"/>
   <pageSetup scale="85" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
@@ -10713,8 +10861,8 @@
   </sheetPr>
   <dimension ref="B2:O50"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I1048576"/>
+    <sheetView topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="R18" sqref="R18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -10730,20 +10878,20 @@
   </cols>
   <sheetData>
     <row r="2" spans="2:15" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="C2" s="285" t="s">
+      <c r="C2" s="287" t="s">
         <v>2</v>
       </c>
-      <c r="D2" s="285"/>
-      <c r="E2" s="285"/>
-      <c r="F2" s="285"/>
-      <c r="G2" s="285"/>
-      <c r="K2" s="311" t="s">
+      <c r="D2" s="287"/>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287"/>
+      <c r="K2" s="330" t="s">
         <v>330</v>
       </c>
-      <c r="L2" s="311"/>
-      <c r="M2" s="311"/>
-      <c r="N2" s="311"/>
-      <c r="O2" s="311"/>
+      <c r="L2" s="330"/>
+      <c r="M2" s="330"/>
+      <c r="N2" s="330"/>
+      <c r="O2" s="330"/>
     </row>
     <row r="3" spans="2:15" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C3" s="43" t="s">
@@ -11572,10 +11720,10 @@
       <c r="G31" s="137"/>
       <c r="J31" s="188"/>
       <c r="K31" s="189"/>
-      <c r="L31" s="312" t="s">
+      <c r="L31" s="313" t="s">
         <v>412</v>
       </c>
-      <c r="M31" s="313"/>
+      <c r="M31" s="314"/>
       <c r="N31" s="185">
         <f>SUM(N4:N30)</f>
         <v>366663.07999999996</v>
@@ -11631,15 +11779,15 @@
     </row>
     <row r="35" spans="2:15" x14ac:dyDescent="0.25">
       <c r="B35" s="112"/>
-      <c r="C35" s="310" t="s">
+      <c r="C35" s="312" t="s">
         <v>210</v>
       </c>
-      <c r="D35" s="310"/>
-      <c r="E35" s="306">
+      <c r="D35" s="312"/>
+      <c r="E35" s="308">
         <f>F32-N31</f>
         <v>851287.64000000025</v>
       </c>
-      <c r="F35" s="307"/>
+      <c r="F35" s="309"/>
       <c r="G35" s="170"/>
       <c r="J35" s="112"/>
       <c r="K35" s="113"/>
@@ -11650,10 +11798,10 @@
     </row>
     <row r="36" spans="2:15" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="112"/>
-      <c r="C36" s="310"/>
-      <c r="D36" s="310"/>
-      <c r="E36" s="308"/>
-      <c r="F36" s="309"/>
+      <c r="C36" s="312"/>
+      <c r="D36" s="312"/>
+      <c r="E36" s="310"/>
+      <c r="F36" s="311"/>
       <c r="G36" s="171"/>
       <c r="J36" s="112"/>
       <c r="K36" s="113"/>
@@ -11781,8 +11929,8 @@
       </c>
       <c r="G44" s="247"/>
       <c r="K44" s="222"/>
-      <c r="L44" s="333"/>
-      <c r="M44" s="333"/>
+      <c r="L44" s="335"/>
+      <c r="M44" s="335"/>
     </row>
     <row r="45" spans="2:15" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D45" s="267">
@@ -11843,10 +11991,10 @@
     </row>
     <row r="49" spans="4:13" ht="21.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="D49" s="252"/>
-      <c r="E49" s="331" t="s">
+      <c r="E49" s="333" t="s">
         <v>464</v>
       </c>
-      <c r="F49" s="329">
+      <c r="F49" s="331">
         <f>SUM(F40:F48)</f>
         <v>0.35999999998603016</v>
       </c>
@@ -11858,8 +12006,8 @@
     </row>
     <row r="50" spans="4:13" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D50" s="254"/>
-      <c r="E50" s="332"/>
-      <c r="F50" s="330"/>
+      <c r="E50" s="334"/>
+      <c r="F50" s="332"/>
       <c r="G50" s="255"/>
       <c r="J50" s="261"/>
       <c r="K50" s="262"/>
@@ -11888,10 +12036,13 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="C2:I50"/>
+  <sheetPr>
+    <tabColor rgb="FFFF00FF"/>
+  </sheetPr>
+  <dimension ref="C2:K51"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView tabSelected="1" topLeftCell="A14" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="R46" sqref="R46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
@@ -11905,16 +12056,16 @@
     <col min="9" max="9" width="7" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="2" spans="3:9" ht="24" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="D2" s="285" t="s">
-        <v>2</v>
-      </c>
-      <c r="E2" s="285"/>
-      <c r="F2" s="285"/>
-      <c r="G2" s="285"/>
-      <c r="H2" s="285"/>
-    </row>
-    <row r="3" spans="3:9" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="2" spans="3:10" ht="24" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D2" s="287" t="s">
+        <v>529</v>
+      </c>
+      <c r="E2" s="287"/>
+      <c r="F2" s="287"/>
+      <c r="G2" s="287"/>
+      <c r="H2" s="287"/>
+    </row>
+    <row r="3" spans="3:10" ht="38.25" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D3" s="43" t="s">
         <v>0</v>
       </c>
@@ -11929,7 +12080,7 @@
       </c>
       <c r="H3" s="44"/>
     </row>
-    <row r="4" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="4" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C4" s="6">
         <v>1</v>
       </c>
@@ -11947,7 +12098,7 @@
       </c>
       <c r="H4" s="136"/>
     </row>
-    <row r="5" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="5" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C5" s="6">
         <v>2</v>
       </c>
@@ -11965,7 +12116,7 @@
       </c>
       <c r="H5" s="137"/>
     </row>
-    <row r="6" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="6" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C6" s="6">
         <v>3</v>
       </c>
@@ -11981,11 +12132,11 @@
       <c r="G6" s="33">
         <v>0</v>
       </c>
-      <c r="H6" s="335" t="s">
+      <c r="H6" s="279" t="s">
         <v>479</v>
       </c>
     </row>
-    <row r="7" spans="3:9" ht="18.75" x14ac:dyDescent="0.3">
+    <row r="7" spans="3:10" ht="18.75" x14ac:dyDescent="0.3">
       <c r="C7" s="6">
         <v>4</v>
       </c>
@@ -12003,7 +12154,7 @@
       </c>
       <c r="H7" s="138"/>
     </row>
-    <row r="8" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="8" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C8" s="6">
         <v>5</v>
       </c>
@@ -12021,7 +12172,7 @@
       </c>
       <c r="H8" s="137"/>
     </row>
-    <row r="9" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="9" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C9" s="6">
         <v>6</v>
       </c>
@@ -12039,7 +12190,7 @@
       </c>
       <c r="H9" s="137"/>
     </row>
-    <row r="10" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="10" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C10" s="6">
         <v>7</v>
       </c>
@@ -12057,7 +12208,7 @@
       </c>
       <c r="H10" s="137"/>
     </row>
-    <row r="11" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="11" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C11" s="6">
         <v>8</v>
       </c>
@@ -12076,9 +12227,10 @@
       <c r="H11" s="336" t="s">
         <v>519</v>
       </c>
-      <c r="I11" s="94"/>
-    </row>
-    <row r="12" spans="3:9" x14ac:dyDescent="0.25">
+      <c r="I11" s="337"/>
+      <c r="J11" s="337"/>
+    </row>
+    <row r="12" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C12" s="6">
         <v>9</v>
       </c>
@@ -12096,7 +12248,7 @@
       </c>
       <c r="H12" s="137"/>
     </row>
-    <row r="13" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="13" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C13" s="6">
         <v>10</v>
       </c>
@@ -12114,7 +12266,7 @@
       </c>
       <c r="H13" s="137"/>
     </row>
-    <row r="14" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="14" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C14" s="6">
         <v>11</v>
       </c>
@@ -12132,7 +12284,7 @@
       </c>
       <c r="H14" s="139"/>
     </row>
-    <row r="15" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="15" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C15" s="6">
         <v>12</v>
       </c>
@@ -12150,7 +12302,7 @@
       </c>
       <c r="H15" s="137"/>
     </row>
-    <row r="16" spans="3:9" x14ac:dyDescent="0.25">
+    <row r="16" spans="3:10" x14ac:dyDescent="0.25">
       <c r="C16" s="6">
         <v>13</v>
       </c>
@@ -12286,9 +12438,11 @@
       <c r="E23" s="105" t="s">
         <v>506</v>
       </c>
-      <c r="F23" s="85"/>
-      <c r="G23" s="10">
-        <v>0</v>
+      <c r="F23" s="30" t="s">
+        <v>520</v>
+      </c>
+      <c r="G23" s="33">
+        <v>13455.2</v>
       </c>
       <c r="H23" s="137"/>
     </row>
@@ -12404,227 +12558,221 @@
       <c r="C30" s="12">
         <v>27</v>
       </c>
-      <c r="D30" s="111"/>
-      <c r="E30" s="40"/>
-      <c r="F30" s="41"/>
-      <c r="G30" s="42"/>
+      <c r="D30" s="111">
+        <v>45255</v>
+      </c>
+      <c r="E30" s="40" t="s">
+        <v>521</v>
+      </c>
+      <c r="F30" s="41" t="s">
+        <v>522</v>
+      </c>
+      <c r="G30" s="42">
+        <v>54408.4</v>
+      </c>
       <c r="H30" s="140"/>
     </row>
     <row r="31" spans="3:8" x14ac:dyDescent="0.25">
-      <c r="C31" s="6"/>
-      <c r="D31" s="32"/>
-      <c r="E31" s="105"/>
-      <c r="F31" s="30"/>
-      <c r="G31" s="33">
-        <v>0</v>
-      </c>
-      <c r="H31" s="137"/>
-    </row>
-    <row r="32" spans="3:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C32" s="112"/>
-      <c r="D32" s="113"/>
-      <c r="E32" s="121" t="s">
-        <v>69</v>
-      </c>
-      <c r="F32" s="122"/>
-      <c r="G32" s="123">
-        <f>SUM(G4:G31)</f>
-        <v>1639202.52</v>
-      </c>
-      <c r="H32" s="141"/>
-    </row>
-    <row r="33" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C31" s="6">
+        <v>28</v>
+      </c>
+      <c r="D31" s="111">
+        <v>45255</v>
+      </c>
+      <c r="E31" s="40" t="s">
+        <v>523</v>
+      </c>
+      <c r="F31" s="41" t="s">
+        <v>524</v>
+      </c>
+      <c r="G31" s="42">
+        <v>28232.7</v>
+      </c>
+      <c r="H31" s="140"/>
+    </row>
+    <row r="32" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="C32" s="12">
+        <v>29</v>
+      </c>
+      <c r="D32" s="32">
+        <v>45255</v>
+      </c>
+      <c r="E32" s="105" t="s">
+        <v>525</v>
+      </c>
+      <c r="F32" s="30" t="s">
+        <v>526</v>
+      </c>
+      <c r="G32" s="33">
+        <v>900</v>
+      </c>
+      <c r="H32" s="137"/>
+    </row>
+    <row r="33" spans="3:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C33" s="112"/>
       <c r="D33" s="113"/>
-      <c r="E33" s="114"/>
-      <c r="F33" s="115"/>
-      <c r="G33" s="116"/>
-      <c r="H33" s="117"/>
-    </row>
-    <row r="34" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E33" s="121" t="s">
+        <v>69</v>
+      </c>
+      <c r="F33" s="122"/>
+      <c r="G33" s="123">
+        <f>SUM(G4:G32)</f>
+        <v>1736198.8199999998</v>
+      </c>
+      <c r="H33" s="141"/>
+    </row>
+    <row r="34" spans="3:11" x14ac:dyDescent="0.25">
       <c r="C34" s="112"/>
-      <c r="D34" s="99"/>
-      <c r="E34" s="100"/>
-      <c r="F34" s="100"/>
-      <c r="G34" s="165"/>
-      <c r="H34" s="169"/>
-    </row>
-    <row r="35" spans="3:8" x14ac:dyDescent="0.25">
+      <c r="D34" s="113"/>
+      <c r="E34" s="114"/>
+      <c r="F34" s="115"/>
+      <c r="G34" s="116"/>
+      <c r="H34" s="117"/>
+    </row>
+    <row r="35" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C35" s="112"/>
-      <c r="D35" s="310" t="s">
+      <c r="D35" s="99"/>
+      <c r="E35" s="100"/>
+      <c r="F35" s="100"/>
+      <c r="G35" s="165"/>
+      <c r="H35" s="169"/>
+    </row>
+    <row r="36" spans="3:11" x14ac:dyDescent="0.25">
+      <c r="C36" s="112"/>
+      <c r="D36" s="312" t="s">
         <v>210</v>
       </c>
-      <c r="E35" s="310"/>
-      <c r="F35" s="306">
-        <f>G32-O31</f>
-        <v>1639202.52</v>
-      </c>
-      <c r="G35" s="307"/>
-      <c r="H35" s="170"/>
-    </row>
-    <row r="36" spans="3:8" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="C36" s="112"/>
-      <c r="D36" s="310"/>
-      <c r="E36" s="310"/>
-      <c r="F36" s="308"/>
+      <c r="E36" s="312"/>
+      <c r="F36" s="308">
+        <f>G33-O32-547174.52</f>
+        <v>1189024.2999999998</v>
+      </c>
       <c r="G36" s="309"/>
-      <c r="H36" s="171"/>
-    </row>
-    <row r="37" spans="3:8" ht="18.75" x14ac:dyDescent="0.25">
+      <c r="H36" s="170"/>
+      <c r="K36" t="s">
+        <v>527</v>
+      </c>
+    </row>
+    <row r="37" spans="3:11" ht="19.5" thickBot="1" x14ac:dyDescent="0.35">
       <c r="C37" s="112"/>
-      <c r="D37" s="99"/>
-      <c r="E37" s="99"/>
-      <c r="F37" s="173" t="s">
-        <v>460</v>
-      </c>
-      <c r="G37" s="173"/>
-      <c r="H37" s="172"/>
-    </row>
-    <row r="38" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D37" s="312"/>
+      <c r="E37" s="312"/>
+      <c r="F37" s="310"/>
+      <c r="G37" s="311"/>
+      <c r="H37" s="171"/>
+    </row>
+    <row r="38" spans="3:11" ht="18.75" x14ac:dyDescent="0.25">
       <c r="C38" s="112"/>
-      <c r="D38" s="86"/>
-      <c r="E38" s="87"/>
-      <c r="F38" s="87"/>
-      <c r="H38" s="119"/>
-    </row>
-    <row r="39" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D38" s="99"/>
+      <c r="E38" s="99"/>
+      <c r="F38" s="173" t="s">
+        <v>528</v>
+      </c>
+      <c r="G38" s="173"/>
+      <c r="H38" s="172"/>
+    </row>
+    <row r="39" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="C39" s="112"/>
-      <c r="E39" s="223" t="s">
+      <c r="D39" s="86"/>
+      <c r="E39" s="87"/>
+      <c r="F39" s="87"/>
+      <c r="H39" s="119"/>
+    </row>
+    <row r="40" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="C40" s="112"/>
+      <c r="E40" s="223" t="s">
         <v>462</v>
       </c>
-      <c r="F39" s="240" t="s">
+      <c r="F40" s="240" t="s">
         <v>461</v>
       </c>
-      <c r="H39" s="118"/>
-    </row>
-    <row r="40" spans="3:8" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="E40" s="241" t="s">
+      <c r="H40" s="118"/>
+    </row>
+    <row r="41" spans="3:11" ht="20.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="E41" s="241" t="s">
         <v>463</v>
       </c>
-      <c r="F40" s="242"/>
-      <c r="G40" s="243">
-        <v>-851287.64</v>
-      </c>
-      <c r="H40" s="244"/>
-    </row>
-    <row r="41" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E41" s="245">
-        <v>45247</v>
-      </c>
-      <c r="F41" s="246">
-        <v>8477</v>
-      </c>
-      <c r="G41" s="184">
-        <v>240040</v>
-      </c>
-      <c r="H41" s="247"/>
-    </row>
-    <row r="42" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E42" s="245">
-        <v>45247</v>
-      </c>
-      <c r="F42" s="246">
-        <v>8484</v>
-      </c>
-      <c r="G42" s="184">
-        <v>100000</v>
-      </c>
+      <c r="F41" s="242"/>
+      <c r="G41" s="243"/>
+      <c r="H41" s="244"/>
+    </row>
+    <row r="42" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E42" s="245"/>
+      <c r="F42" s="246"/>
+      <c r="G42" s="184"/>
       <c r="H42" s="247"/>
     </row>
-    <row r="43" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E43" s="245">
-        <v>45247</v>
-      </c>
-      <c r="F43" s="246">
-        <v>8485</v>
-      </c>
-      <c r="G43" s="184">
-        <v>100000</v>
-      </c>
+    <row r="43" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E43" s="245"/>
+      <c r="F43" s="246"/>
+      <c r="G43" s="184"/>
       <c r="H43" s="247"/>
     </row>
-    <row r="44" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E44" s="245">
-        <v>45247</v>
-      </c>
-      <c r="F44" s="246">
-        <v>8486</v>
-      </c>
-      <c r="G44" s="184">
-        <v>100000</v>
-      </c>
+    <row r="44" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E44" s="245"/>
+      <c r="F44" s="246"/>
+      <c r="G44" s="184"/>
       <c r="H44" s="247"/>
     </row>
-    <row r="45" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E45" s="267">
-        <v>45251</v>
-      </c>
-      <c r="F45" s="268">
-        <v>8514</v>
-      </c>
-      <c r="G45" s="269">
-        <v>150000</v>
-      </c>
-      <c r="H45" s="270"/>
-    </row>
-    <row r="46" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E46" s="267">
-        <v>45251</v>
-      </c>
-      <c r="F46" s="268">
-        <v>8531</v>
-      </c>
-      <c r="G46" s="269">
-        <v>21248</v>
-      </c>
+    <row r="45" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E45" s="245"/>
+      <c r="F45" s="246"/>
+      <c r="G45" s="184"/>
+      <c r="H45" s="247"/>
+    </row>
+    <row r="46" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E46" s="267"/>
+      <c r="F46" s="268"/>
+      <c r="G46" s="269"/>
       <c r="H46" s="270"/>
     </row>
-    <row r="47" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E47" s="267">
-        <v>45251</v>
-      </c>
-      <c r="F47" s="268">
-        <v>8532</v>
-      </c>
-      <c r="G47" s="269">
-        <v>140000</v>
-      </c>
+    <row r="47" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E47" s="267"/>
+      <c r="F47" s="268"/>
+      <c r="G47" s="269"/>
       <c r="H47" s="270"/>
     </row>
-    <row r="48" spans="3:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E48" s="248"/>
-      <c r="F48" s="249"/>
-      <c r="G48" s="250">
+    <row r="48" spans="3:11" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E48" s="267"/>
+      <c r="F48" s="268"/>
+      <c r="G48" s="269"/>
+      <c r="H48" s="270"/>
+    </row>
+    <row r="49" spans="5:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E49" s="248"/>
+      <c r="F49" s="249"/>
+      <c r="G49" s="250">
         <v>0</v>
       </c>
-      <c r="H48" s="251"/>
-    </row>
-    <row r="49" spans="5:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="E49" s="252"/>
-      <c r="F49" s="331" t="s">
+      <c r="H49" s="251"/>
+    </row>
+    <row r="50" spans="5:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="E50" s="252"/>
+      <c r="F50" s="333" t="s">
         <v>464</v>
       </c>
-      <c r="G49" s="329">
-        <f>SUM(G40:G48)</f>
-        <v>0.35999999998603016</v>
-      </c>
-      <c r="H49" s="253"/>
-    </row>
-    <row r="50" spans="5:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="E50" s="254"/>
-      <c r="F50" s="332"/>
-      <c r="G50" s="330"/>
-      <c r="H50" s="255"/>
+      <c r="G50" s="331">
+        <f>SUM(G41:G49)</f>
+        <v>0</v>
+      </c>
+      <c r="H50" s="253"/>
+    </row>
+    <row r="51" spans="5:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="E51" s="254"/>
+      <c r="F51" s="334"/>
+      <c r="G51" s="332"/>
+      <c r="H51" s="255"/>
     </row>
   </sheetData>
   <mergeCells count="5">
     <mergeCell ref="D2:H2"/>
-    <mergeCell ref="D35:E36"/>
-    <mergeCell ref="F35:G36"/>
-    <mergeCell ref="F49:F50"/>
-    <mergeCell ref="G49:G50"/>
+    <mergeCell ref="D36:E37"/>
+    <mergeCell ref="F36:G37"/>
+    <mergeCell ref="F50:F51"/>
+    <mergeCell ref="G50:G51"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 

</xml_diff>